<commit_message>
Updates from Professor feedback
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnguyen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnguyen/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{976FC51F-BB20-CB45-BAD1-040AD9EE37F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6DE111-2FEB-954C-96A6-31F30B9F33FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16260" yWindow="1240" windowWidth="20580" windowHeight="18260" xr2:uid="{6769108C-C0D1-7F48-99CB-B1D9029DCB44}"/>
+    <workbookView xWindow="39300" yWindow="-7460" windowWidth="21260" windowHeight="10080" xr2:uid="{6769108C-C0D1-7F48-99CB-B1D9029DCB44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,9 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Winogrande</t>
-  </si>
-  <si>
-    <t>Arc_challenge</t>
-  </si>
-  <si>
     <t>gemma-2b</t>
   </si>
   <si>
-    <t>Qlora</t>
-  </si>
-  <si>
     <t>Flash Attention 2</t>
   </si>
   <si>
@@ -75,16 +66,32 @@
   </si>
   <si>
     <t>Inference Memory (MiB)</t>
+  </si>
+  <si>
+    <t>Winogrande (Accuracy %)</t>
+  </si>
+  <si>
+    <t>Arc_challenge (Accuracy %)</t>
+  </si>
+  <si>
+    <t>QLora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAAF06-DD31-4142-9CB2-54B5025E06D3}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -459,7 +467,8 @@
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -467,27 +476,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>2.5099999999999998</v>
@@ -510,7 +519,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2.5099999999999998</v>
@@ -533,7 +542,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1.55</v>
@@ -556,7 +565,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2.5099999999999998</v>
@@ -579,48 +588,48 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>1.57</v>
       </c>
       <c r="C6">
-        <v>3.2</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="D6">
-        <v>12.007</v>
+        <v>10.975</v>
       </c>
       <c r="E6">
-        <v>5862.96</v>
+        <v>1813.21</v>
       </c>
       <c r="F6">
-        <v>0.49490000000000001</v>
+        <v>0.63690000000000002</v>
       </c>
       <c r="G6">
-        <v>0.26019999999999999</v>
+        <v>0.4249</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>1.57</v>
-      </c>
-      <c r="C7">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="D7">
-        <v>10.975</v>
-      </c>
-      <c r="E7">
-        <v>5028.16</v>
-      </c>
-      <c r="F7">
-        <v>0.63690000000000002</v>
-      </c>
-      <c r="G7">
-        <v>0.4249</v>
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.55</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3.14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>13.023999999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3340.33</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.49009000000000003</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.22009999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>